<commit_message>
Nội dung commit mà bạn thêm hoặc sửa
</commit_message>
<xml_diff>
--- a/target/test-classes/testdata/GetProductInfo1.xlsx
+++ b/target/test-classes/testdata/GetProductInfo1.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>50.000 VND</t>
+  </si>
+  <si>
+    <t>22</t>
   </si>
 </sst>
 </file>
@@ -204,8 +207,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -855,7 +873,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E14CBE7-7DC6-4015-BE70-B317C0059D6C}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
@@ -1243,6 +1261,23 @@
         <v>9</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="s" s="106">
+        <v>43</v>
+      </c>
+      <c r="B23" t="s" s="107">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s" s="108">
+        <v>14</v>
+      </c>
+      <c r="D23" t="s" s="109">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s" s="110">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>